<commit_message>
Atualiza instrução de trabalho
</commit_message>
<xml_diff>
--- a/Base/Backlog_11.xlsx
+++ b/Base/Backlog_11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D142BB23-4FCA-4329-9F32-A89101D4503F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F3C125-0BB6-4BE3-8E4C-21195C65B274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" activeTab="1" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
@@ -115,10 +115,10 @@
     <t>Alana Neris</t>
   </si>
   <si>
-    <t>Erick Silva</t>
-  </si>
-  <si>
     <t>Resolvido</t>
+  </si>
+  <si>
+    <t>Erick da Silva</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
         <v>45733</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>21</v>
@@ -802,11 +802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="B25" sqref="B24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -861,7 +860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -890,13 +889,13 @@
         <v>45733</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -925,13 +924,13 @@
         <v>45733</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -960,13 +959,13 @@
         <v>45733</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -995,13 +994,13 @@
         <v>45733</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -1030,13 +1029,13 @@
         <v>45733</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
@@ -1065,13 +1064,13 @@
         <v>45733</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
@@ -1100,18 +1099,18 @@
         <v>45733</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="15">
         <v>2025</v>
@@ -1135,18 +1134,18 @@
         <v>45733</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="15">
         <v>2025</v>
@@ -1170,18 +1169,18 @@
         <v>45733</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="15">
         <v>2025</v>
@@ -1246,7 +1245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
@@ -1275,13 +1274,13 @@
         <v>45733</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>4</v>
       </c>
@@ -1310,13 +1309,13 @@
         <v>45733</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>4</v>
       </c>
@@ -1345,7 +1344,7 @@
         <v>45733</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>11</v>
@@ -1386,7 +1385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>45733</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>11</v>
@@ -1456,7 +1455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>4</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>4</v>
       </c>
@@ -1520,13 +1519,13 @@
         <v>45733</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
@@ -1555,13 +1554,13 @@
         <v>45733</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="20" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1640,7 +1639,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1649,7 +1648,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1658,7 +1657,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="12"/>
@@ -1666,7 +1665,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1675,7 +1674,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1684,7 +1683,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="12"/>
@@ -1692,7 +1691,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="12"/>
@@ -1700,7 +1699,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="12"/>
@@ -1708,7 +1707,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="13"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1717,7 +1716,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="13"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1726,7 +1725,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1735,7 +1734,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1744,7 +1743,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="13"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1753,7 +1752,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1762,7 +1761,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="3"/>
@@ -1773,7 +1772,7 @@
       <c r="I39" s="9"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="3"/>
@@ -1784,7 +1783,7 @@
       <c r="I40" s="9"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="3"/>
@@ -1795,7 +1794,7 @@
       <c r="I41" s="9"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="3"/>
@@ -1806,7 +1805,7 @@
       <c r="I42" s="9"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="3"/>
@@ -1817,7 +1816,7 @@
       <c r="I43" s="9"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="3"/>
@@ -1828,7 +1827,7 @@
       <c r="I44" s="9"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="3"/>
@@ -1839,7 +1838,7 @@
       <c r="I45" s="9"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="3"/>
@@ -1850,7 +1849,7 @@
       <c r="I46" s="9"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="3"/>
@@ -1861,7 +1860,7 @@
       <c r="I47" s="9"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="3"/>
@@ -1872,7 +1871,7 @@
       <c r="I48" s="9"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="3"/>
@@ -1883,7 +1882,7 @@
       <c r="I49" s="9"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="3"/>
@@ -2217,18 +2216,7 @@
       <c r="I93" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J50" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
-    <filterColumn colId="7">
-      <filters>
-        <dateGroupItem year="2025" month="2" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Pendente"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J50" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>